<commit_message>
mustafa | correct import sample file
</commit_message>
<xml_diff>
--- a/src/assets/sample-files/account-sample.xlsx
+++ b/src/assets/sample-files/account-sample.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubhendra\Desktop\GST\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACBBD92B-C96B-4884-B0B3-6CB14138CB85}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
   <si>
     <t>name</t>
   </si>
@@ -104,25 +113,129 @@
   </si>
   <si>
     <t>akshay1</t>
+  </si>
+  <si>
+    <t>rahul dev</t>
+  </si>
+  <si>
+    <t>rahul123</t>
+  </si>
+  <si>
+    <t>rahultest@walkovertest1</t>
+  </si>
+  <si>
+    <t>rdrahul</t>
+  </si>
+  <si>
+    <t>devesh jha</t>
+  </si>
+  <si>
+    <t>devj34</t>
+  </si>
+  <si>
+    <t>Sundry Creditors</t>
+  </si>
+  <si>
+    <t>devesh@walkovertest1</t>
+  </si>
+  <si>
+    <t>jha devesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aditya singh </t>
+  </si>
+  <si>
+    <t>adisg3t</t>
+  </si>
+  <si>
+    <t>adi@walkovertest1</t>
+  </si>
+  <si>
+    <t>adi to</t>
+  </si>
+  <si>
+    <t>kamal rajni</t>
+  </si>
+  <si>
+    <t>kamal45</t>
+  </si>
+  <si>
+    <t>kamal@walkovertest1</t>
+  </si>
+  <si>
+    <t>kamalrj</t>
+  </si>
+  <si>
+    <t>hitesh kumar</t>
+  </si>
+  <si>
+    <t>hitkum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sundry Debtors </t>
+  </si>
+  <si>
+    <t>hitesh@walkovertest1</t>
+  </si>
+  <si>
+    <t>hitkumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeetu </t>
+  </si>
+  <si>
+    <t>jeet2</t>
+  </si>
+  <si>
+    <t>jeet@walkovertest1</t>
+  </si>
+  <si>
+    <t>sachin</t>
+  </si>
+  <si>
+    <t>abhishek</t>
+  </si>
+  <si>
+    <t>abhi23</t>
+  </si>
+  <si>
+    <t>DEBIT</t>
+  </si>
+  <si>
+    <t>abhi@walkovertest1</t>
+  </si>
+  <si>
+    <t>abhiranjan</t>
+  </si>
+  <si>
+    <t>GST231111111111111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -131,11 +244,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -149,50 +268,357 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -248,7 +674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -262,16 +688,16 @@
         <v>21</v>
       </c>
       <c r="E2" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F2" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="G2" s="3">
-        <v>9.479400728E9</v>
+        <v>8889378604</v>
       </c>
       <c r="H2" s="3">
-        <v>91.0</v>
+        <v>91</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>22</v>
@@ -288,11 +714,11 @@
       <c r="M2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="2">
-        <v>2.31111111111111E14</v>
+      <c r="N2" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="O2" s="3">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="P2" s="4" t="b">
         <v>0</v>
@@ -304,7 +730,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -318,16 +744,16 @@
         <v>21</v>
       </c>
       <c r="E3" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F3" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="G3" s="3">
-        <v>9.479400728E9</v>
+        <v>8889378602</v>
       </c>
       <c r="H3" s="3">
-        <v>91.0</v>
+        <v>91</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>22</v>
@@ -344,11 +770,11 @@
       <c r="M3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="2">
-        <v>2.31111111111111E14</v>
+      <c r="N3" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="O3" s="3">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="P3" s="4" t="b">
         <v>0</v>
@@ -360,7 +786,411 @@
         <v>28</v>
       </c>
     </row>
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4" s="3">
+        <v>8889378605</v>
+      </c>
+      <c r="H4">
+        <v>91</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4">
+        <v>23</v>
+      </c>
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5" s="3">
+        <v>8889378603</v>
+      </c>
+      <c r="H5">
+        <v>91</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O5">
+        <v>23</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>27</v>
+      </c>
+      <c r="R5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>8818888761</v>
+      </c>
+      <c r="H6">
+        <v>91</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6">
+        <v>23</v>
+      </c>
+      <c r="P6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7" s="3">
+        <v>8889378604</v>
+      </c>
+      <c r="H7">
+        <v>91</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7">
+        <v>23</v>
+      </c>
+      <c r="P7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>27</v>
+      </c>
+      <c r="R7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8" s="3">
+        <v>8889378604</v>
+      </c>
+      <c r="H8">
+        <v>91</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8">
+        <v>23</v>
+      </c>
+      <c r="P8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9" s="3">
+        <v>8889378604</v>
+      </c>
+      <c r="H9">
+        <v>91</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O9">
+        <v>33</v>
+      </c>
+      <c r="P9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>27</v>
+      </c>
+      <c r="R9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>2000</v>
+      </c>
+      <c r="G10" s="3">
+        <v>8889378604</v>
+      </c>
+      <c r="H10">
+        <v>91</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O10">
+        <v>37</v>
+      </c>
+      <c r="P10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>27</v>
+      </c>
+      <c r="R10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H14" s="3"/>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{80677539-D13E-4E75-88B5-8808DF566CC5}"/>
+    <hyperlink ref="I5" r:id="rId2" xr:uid="{A4836677-9C1B-4406-8EE4-BEF20F703A03}"/>
+    <hyperlink ref="I6" r:id="rId3" xr:uid="{B48FF2C5-D73E-4C8F-B918-73F54077D5DB}"/>
+    <hyperlink ref="I7" r:id="rId4" xr:uid="{3E223E50-796C-4CA3-B2FF-098DE44DAD7A}"/>
+    <hyperlink ref="I8" r:id="rId5" xr:uid="{824FCDD3-2E25-4E60-8650-83A5F2591E04}"/>
+    <hyperlink ref="I9" r:id="rId6" xr:uid="{0CAE6120-8299-4BB1-86F4-B20F39AF6E96}"/>
+    <hyperlink ref="I10" r:id="rId7" xr:uid="{9A7E7A0F-57CD-4270-8D1E-397B4FC24A5D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
replacing old sample files in import module
</commit_message>
<xml_diff>
--- a/src/assets/sample-files/account-sample.xlsx
+++ b/src/assets/sample-files/account-sample.xlsx
@@ -179,7 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -192,15 +192,14 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
-    </font>
-    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,14 +212,8 @@
         <bgColor rgb="FFFFF6F1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border/>
     <border>
       <left style="thin">
@@ -232,6 +225,42 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -240,39 +269,48 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -296,138 +334,113 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.0"/>
-    <col customWidth="1" min="2" max="2" width="17.71"/>
-    <col customWidth="1" min="3" max="3" width="21.0"/>
-    <col customWidth="1" min="4" max="4" width="14.71"/>
-    <col customWidth="1" min="5" max="5" width="14.0"/>
-    <col customWidth="1" min="6" max="6" width="11.29"/>
-    <col customWidth="1" min="7" max="7" width="11.43"/>
-    <col customWidth="1" min="8" max="8" width="18.14"/>
-    <col customWidth="1" min="9" max="9" width="13.0"/>
-    <col customWidth="1" min="10" max="10" width="11.43"/>
-    <col customWidth="1" min="11" max="11" width="18.14"/>
-    <col customWidth="1" min="12" max="12" width="22.0"/>
-    <col customWidth="1" min="13" max="13" width="19.71"/>
-    <col customWidth="1" min="14" max="14" width="17.29"/>
-    <col customWidth="1" min="15" max="15" width="13.0"/>
-    <col customWidth="1" min="16" max="16" width="13.57"/>
     <col customWidth="1" min="17" max="17" width="17.0"/>
   </cols>
   <sheetData>
-    <row r="1" ht="48.0" customHeight="1">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="6">
         <v>23.0</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="6">
         <v>91.0</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="8">
         <v>8.818888764E9</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="6">
         <v>0.0</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="6">
         <v>100.0</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+      <c r="P2" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -439,20 +452,20 @@
       <c r="D3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="E3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="11">
         <v>7.0</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="11">
         <v>91.0</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="12">
         <v>8.818888768E9</v>
       </c>
       <c r="K3" s="7" t="s">
@@ -461,22 +474,22 @@
       <c r="L3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="11">
         <v>0.0</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="11">
         <v>500.0</v>
       </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="3" t="s">
+      <c r="O3" s="7"/>
+      <c r="P3" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -486,32 +499,32 @@
         <v>35</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="E4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="11">
         <v>23.0</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="8"/>
+      <c r="I4" s="11"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
       <c r="O4" s="7"/>
-      <c r="P4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="3" t="s">
+      <c r="P4" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -520,33 +533,33 @@
       <c r="C5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="D5" s="7"/>
+      <c r="E5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="11">
         <v>23.0</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="3" t="s">
+      <c r="I5" s="11"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -555,33 +568,33 @@
       <c r="C6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="8">
+      <c r="D6" s="7"/>
+      <c r="E6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="11">
         <v>1.0</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="7" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3" t="s">
+      <c r="I6" s="11"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -593,38 +606,38 @@
       <c r="D7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="E7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="11">
         <v>23.0</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="11">
         <v>91.0</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="12">
         <v>1.23456789E9</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="13" t="s">
         <v>45</v>
       </c>
       <c r="L7" s="7"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="3" t="s">
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -633,31 +646,31 @@
       <c r="C8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="8">
+      <c r="D8" s="7"/>
+      <c r="E8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="11">
         <v>23.0</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="3" t="s">
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -666,31 +679,31 @@
       <c r="C9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="8">
+      <c r="D9" s="7"/>
+      <c r="E9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="11">
         <v>23.0</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="3" t="s">
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -699,85 +712,28 @@
       <c r="C10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="D10" s="7"/>
+      <c r="E10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="11">
         <v>23.0</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>